<commit_message>
Changes to school costs index chart
</commit_message>
<xml_diff>
--- a/data/school_costs/school costs.xlsx
+++ b/data/school_costs/school costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awby\github\school-cuts\data\school_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684C5C57-EC17-489C-84AD-F12B9C6A89E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC34818-B27B-4E12-9AB2-4B789F7C43AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1402,20 +1402,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1438,10 +1435,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1449,9 +1452,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1504,7 +1504,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="l">
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1517,12 +1517,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+              <a:rPr lang="en-GB" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Cumulative cost pressures for schools, 2010-11 to 2023-24</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB" sz="1400">
+            <a:endParaRPr lang="en-GB" sz="1400" b="1">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1549,7 +1549,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l">
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1573,9 +1573,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13144046504048151"/>
-          <c:y val="0.16740972033668203"/>
+          <c:y val="0.12195058192854762"/>
           <c:w val="0.86287367725459929"/>
-          <c:h val="0.60840803692641865"/>
+          <c:h val="0.65386719258022785"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2829,10 +2829,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2926,8 +2923,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="4.7585962904484261E-2"/>
-              <c:y val="0.1043770019085082"/>
+              <c:x val="7.2224782025974196E-2"/>
+              <c:y val="7.2693369391184259E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3027,7 +3024,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5097,10 +5094,10 @@
         <f t="shared" si="12"/>
         <v>4.8581487479021121E-2</v>
       </c>
-      <c r="F43" s="108"/>
-      <c r="G43" s="108"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="108"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="92"/>
+      <c r="H43" s="92"/>
+      <c r="I43" s="92"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="str">
@@ -5119,10 +5116,10 @@
         <f t="shared" si="12"/>
         <v>4.8054703028083873E-2</v>
       </c>
-      <c r="F44" s="108"/>
-      <c r="G44" s="108"/>
-      <c r="H44" s="108"/>
-      <c r="I44" s="108"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
@@ -6253,68 +6250,68 @@
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="93" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="94" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="96"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="73"/>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="98"/>
     </row>
     <row r="6" spans="1:13" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="91"/>
       <c r="B6" s="72"/>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="101"/>
+      <c r="D6" s="100"/>
       <c r="E6" s="71" t="s">
         <v>176</v>
       </c>
       <c r="F6" s="70"/>
       <c r="G6" s="91"/>
       <c r="H6" s="69"/>
-      <c r="I6" s="102" t="s">
+      <c r="I6" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="J6" s="103"/>
+      <c r="J6" s="102"/>
       <c r="K6" s="68" t="s">
         <v>174</v>
       </c>
@@ -8719,109 +8716,109 @@
       <c r="B81" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="105" t="s">
+      <c r="C81" s="95" t="s">
         <v>211</v>
       </c>
-      <c r="D81" s="105"/>
-      <c r="E81" s="105"/>
-      <c r="F81" s="105"/>
-      <c r="G81" s="105"/>
-      <c r="H81" s="105"/>
-      <c r="I81" s="105"/>
-      <c r="J81" s="105"/>
-      <c r="K81" s="105"/>
+      <c r="D81" s="95"/>
+      <c r="E81" s="95"/>
+      <c r="F81" s="95"/>
+      <c r="G81" s="95"/>
+      <c r="H81" s="95"/>
+      <c r="I81" s="95"/>
+      <c r="J81" s="95"/>
+      <c r="K81" s="95"/>
     </row>
     <row r="82" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="30"/>
       <c r="B82" s="32"/>
-      <c r="C82" s="104" t="s">
+      <c r="C82" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="D82" s="105"/>
-      <c r="E82" s="105"/>
-      <c r="F82" s="105"/>
-      <c r="G82" s="105"/>
-      <c r="H82" s="105"/>
-      <c r="I82" s="105"/>
-      <c r="J82" s="105"/>
-      <c r="K82" s="105"/>
+      <c r="D82" s="95"/>
+      <c r="E82" s="95"/>
+      <c r="F82" s="95"/>
+      <c r="G82" s="95"/>
+      <c r="H82" s="95"/>
+      <c r="I82" s="95"/>
+      <c r="J82" s="95"/>
+      <c r="K82" s="95"/>
     </row>
     <row r="83" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="30"/>
       <c r="B83" s="32"/>
-      <c r="C83" s="105" t="s">
+      <c r="C83" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="D83" s="105"/>
-      <c r="E83" s="105"/>
-      <c r="F83" s="105"/>
-      <c r="G83" s="105"/>
-      <c r="H83" s="105"/>
-      <c r="I83" s="105"/>
-      <c r="J83" s="105"/>
-      <c r="K83" s="105"/>
+      <c r="D83" s="95"/>
+      <c r="E83" s="95"/>
+      <c r="F83" s="95"/>
+      <c r="G83" s="95"/>
+      <c r="H83" s="95"/>
+      <c r="I83" s="95"/>
+      <c r="J83" s="95"/>
+      <c r="K83" s="95"/>
     </row>
     <row r="84" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="30"/>
       <c r="B84" s="32"/>
-      <c r="C84" s="104" t="s">
+      <c r="C84" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="D84" s="105"/>
-      <c r="E84" s="105"/>
-      <c r="F84" s="105"/>
-      <c r="G84" s="105"/>
-      <c r="H84" s="105"/>
-      <c r="I84" s="105"/>
-      <c r="J84" s="105"/>
-      <c r="K84" s="105"/>
+      <c r="D84" s="95"/>
+      <c r="E84" s="95"/>
+      <c r="F84" s="95"/>
+      <c r="G84" s="95"/>
+      <c r="H84" s="95"/>
+      <c r="I84" s="95"/>
+      <c r="J84" s="95"/>
+      <c r="K84" s="95"/>
     </row>
     <row r="85" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="30"/>
       <c r="B85" s="32"/>
-      <c r="C85" s="106" t="s">
+      <c r="C85" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="D85" s="106"/>
-      <c r="E85" s="106"/>
-      <c r="F85" s="106"/>
-      <c r="G85" s="106"/>
-      <c r="H85" s="106"/>
-      <c r="I85" s="106"/>
-      <c r="J85" s="106"/>
-      <c r="K85" s="106"/>
+      <c r="D85" s="107"/>
+      <c r="E85" s="107"/>
+      <c r="F85" s="107"/>
+      <c r="G85" s="107"/>
+      <c r="H85" s="107"/>
+      <c r="I85" s="107"/>
+      <c r="J85" s="107"/>
+      <c r="K85" s="107"/>
     </row>
     <row r="86" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="30"/>
       <c r="B86" s="32"/>
-      <c r="C86" s="104" t="s">
+      <c r="C86" s="106" t="s">
         <v>198</v>
       </c>
-      <c r="D86" s="105"/>
-      <c r="E86" s="105"/>
-      <c r="F86" s="105"/>
-      <c r="G86" s="105"/>
-      <c r="H86" s="105"/>
-      <c r="I86" s="105"/>
-      <c r="J86" s="105"/>
-      <c r="K86" s="105"/>
+      <c r="D86" s="95"/>
+      <c r="E86" s="95"/>
+      <c r="F86" s="95"/>
+      <c r="G86" s="95"/>
+      <c r="H86" s="95"/>
+      <c r="I86" s="95"/>
+      <c r="J86" s="95"/>
+      <c r="K86" s="95"/>
     </row>
     <row r="87" spans="1:16" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="30"/>
       <c r="B87" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C87" s="105" t="s">
+      <c r="C87" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="D87" s="105"/>
-      <c r="E87" s="105"/>
-      <c r="F87" s="105"/>
-      <c r="G87" s="105"/>
-      <c r="H87" s="105"/>
-      <c r="I87" s="105"/>
-      <c r="J87" s="105"/>
-      <c r="K87" s="105"/>
+      <c r="D87" s="95"/>
+      <c r="E87" s="95"/>
+      <c r="F87" s="95"/>
+      <c r="G87" s="95"/>
+      <c r="H87" s="95"/>
+      <c r="I87" s="95"/>
+      <c r="J87" s="95"/>
+      <c r="K87" s="95"/>
       <c r="M87" s="31"/>
       <c r="N87" s="31"/>
       <c r="P87" s="31"/>
@@ -8829,32 +8826,32 @@
     <row r="88" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
       <c r="B88" s="32"/>
-      <c r="C88" s="104" t="s">
+      <c r="C88" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="D88" s="105"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="105"/>
-      <c r="G88" s="105"/>
-      <c r="H88" s="105"/>
-      <c r="I88" s="105"/>
-      <c r="J88" s="105"/>
-      <c r="K88" s="105"/>
+      <c r="D88" s="95"/>
+      <c r="E88" s="95"/>
+      <c r="F88" s="95"/>
+      <c r="G88" s="95"/>
+      <c r="H88" s="95"/>
+      <c r="I88" s="95"/>
+      <c r="J88" s="95"/>
+      <c r="K88" s="95"/>
     </row>
     <row r="89" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="30"/>
       <c r="B89" s="32"/>
-      <c r="C89" s="105" t="s">
+      <c r="C89" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="D89" s="105"/>
-      <c r="E89" s="105"/>
-      <c r="F89" s="105"/>
-      <c r="G89" s="105"/>
-      <c r="H89" s="105"/>
-      <c r="I89" s="105"/>
-      <c r="J89" s="105"/>
-      <c r="K89" s="105"/>
+      <c r="D89" s="95"/>
+      <c r="E89" s="95"/>
+      <c r="F89" s="95"/>
+      <c r="G89" s="95"/>
+      <c r="H89" s="95"/>
+      <c r="I89" s="95"/>
+      <c r="J89" s="95"/>
+      <c r="K89" s="95"/>
       <c r="M89" s="31"/>
       <c r="N89" s="31"/>
       <c r="P89" s="31"/>
@@ -8862,47 +8859,47 @@
     <row r="90" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="30"/>
       <c r="B90" s="32"/>
-      <c r="C90" s="104" t="s">
+      <c r="C90" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="D90" s="105"/>
-      <c r="E90" s="105"/>
-      <c r="F90" s="105"/>
-      <c r="G90" s="105"/>
-      <c r="H90" s="105"/>
-      <c r="I90" s="105"/>
-      <c r="J90" s="105"/>
-      <c r="K90" s="105"/>
+      <c r="D90" s="95"/>
+      <c r="E90" s="95"/>
+      <c r="F90" s="95"/>
+      <c r="G90" s="95"/>
+      <c r="H90" s="95"/>
+      <c r="I90" s="95"/>
+      <c r="J90" s="95"/>
+      <c r="K90" s="95"/>
     </row>
     <row r="91" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="30"/>
       <c r="B91" s="32"/>
-      <c r="C91" s="106" t="s">
+      <c r="C91" s="107" t="s">
         <v>205</v>
       </c>
-      <c r="D91" s="106"/>
-      <c r="E91" s="106"/>
-      <c r="F91" s="106"/>
-      <c r="G91" s="106"/>
-      <c r="H91" s="106"/>
-      <c r="I91" s="106"/>
-      <c r="J91" s="106"/>
-      <c r="K91" s="106"/>
+      <c r="D91" s="107"/>
+      <c r="E91" s="107"/>
+      <c r="F91" s="107"/>
+      <c r="G91" s="107"/>
+      <c r="H91" s="107"/>
+      <c r="I91" s="107"/>
+      <c r="J91" s="107"/>
+      <c r="K91" s="107"/>
     </row>
     <row r="92" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="30"/>
       <c r="B92" s="32"/>
-      <c r="C92" s="104" t="s">
+      <c r="C92" s="106" t="s">
         <v>198</v>
       </c>
-      <c r="D92" s="105"/>
-      <c r="E92" s="105"/>
-      <c r="F92" s="105"/>
-      <c r="G92" s="105"/>
-      <c r="H92" s="105"/>
-      <c r="I92" s="105"/>
-      <c r="J92" s="105"/>
-      <c r="K92" s="105"/>
+      <c r="D92" s="95"/>
+      <c r="E92" s="95"/>
+      <c r="F92" s="95"/>
+      <c r="G92" s="95"/>
+      <c r="H92" s="95"/>
+      <c r="I92" s="95"/>
+      <c r="J92" s="95"/>
+      <c r="K92" s="95"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="30"/>
@@ -8923,17 +8920,17 @@
       <c r="B94" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C94" s="107" t="s">
+      <c r="C94" s="108" t="s">
         <v>204</v>
       </c>
-      <c r="D94" s="107"/>
-      <c r="E94" s="107"/>
-      <c r="F94" s="107"/>
-      <c r="G94" s="107"/>
-      <c r="H94" s="107"/>
-      <c r="I94" s="107"/>
-      <c r="J94" s="107"/>
-      <c r="K94" s="107"/>
+      <c r="D94" s="108"/>
+      <c r="E94" s="108"/>
+      <c r="F94" s="108"/>
+      <c r="G94" s="108"/>
+      <c r="H94" s="108"/>
+      <c r="I94" s="108"/>
+      <c r="J94" s="108"/>
+      <c r="K94" s="108"/>
       <c r="M94" s="31"/>
       <c r="N94" s="31"/>
       <c r="P94" s="31"/>
@@ -8942,17 +8939,17 @@
       <c r="B95" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C95" s="105" t="s">
+      <c r="C95" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="D95" s="105"/>
-      <c r="E95" s="105"/>
-      <c r="F95" s="105"/>
-      <c r="G95" s="105"/>
-      <c r="H95" s="105"/>
-      <c r="I95" s="105"/>
-      <c r="J95" s="105"/>
-      <c r="K95" s="105"/>
+      <c r="D95" s="95"/>
+      <c r="E95" s="95"/>
+      <c r="F95" s="95"/>
+      <c r="G95" s="95"/>
+      <c r="H95" s="95"/>
+      <c r="I95" s="95"/>
+      <c r="J95" s="95"/>
+      <c r="K95" s="95"/>
       <c r="M95" s="31"/>
       <c r="N95" s="31"/>
       <c r="P95" s="31"/>
@@ -8961,17 +8958,17 @@
       <c r="B96" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C96" s="105" t="s">
+      <c r="C96" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="D96" s="105"/>
-      <c r="E96" s="105"/>
-      <c r="F96" s="105"/>
-      <c r="G96" s="105"/>
-      <c r="H96" s="105"/>
-      <c r="I96" s="105"/>
-      <c r="J96" s="105"/>
-      <c r="K96" s="105"/>
+      <c r="D96" s="95"/>
+      <c r="E96" s="95"/>
+      <c r="F96" s="95"/>
+      <c r="G96" s="95"/>
+      <c r="H96" s="95"/>
+      <c r="I96" s="95"/>
+      <c r="J96" s="95"/>
+      <c r="K96" s="95"/>
       <c r="M96" s="31"/>
       <c r="N96" s="31"/>
       <c r="P96" s="31"/>
@@ -8980,17 +8977,17 @@
       <c r="B97" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C97" s="105" t="s">
+      <c r="C97" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="D97" s="105"/>
-      <c r="E97" s="105"/>
-      <c r="F97" s="105"/>
-      <c r="G97" s="105"/>
-      <c r="H97" s="105"/>
-      <c r="I97" s="105"/>
-      <c r="J97" s="105"/>
-      <c r="K97" s="105"/>
+      <c r="D97" s="95"/>
+      <c r="E97" s="95"/>
+      <c r="F97" s="95"/>
+      <c r="G97" s="95"/>
+      <c r="H97" s="95"/>
+      <c r="I97" s="95"/>
+      <c r="J97" s="95"/>
+      <c r="K97" s="95"/>
       <c r="M97" s="31"/>
       <c r="N97" s="31"/>
       <c r="P97" s="31"/>
@@ -8999,17 +8996,17 @@
       <c r="B98" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C98" s="105" t="s">
+      <c r="C98" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="D98" s="105"/>
-      <c r="E98" s="105"/>
-      <c r="F98" s="105"/>
-      <c r="G98" s="105"/>
-      <c r="H98" s="105"/>
-      <c r="I98" s="105"/>
-      <c r="J98" s="105"/>
-      <c r="K98" s="105"/>
+      <c r="D98" s="95"/>
+      <c r="E98" s="95"/>
+      <c r="F98" s="95"/>
+      <c r="G98" s="95"/>
+      <c r="H98" s="95"/>
+      <c r="I98" s="95"/>
+      <c r="J98" s="95"/>
+      <c r="K98" s="95"/>
       <c r="M98" s="31"/>
       <c r="N98" s="31"/>
       <c r="P98" s="31"/>
@@ -9017,17 +9014,17 @@
     <row r="99" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="30"/>
       <c r="B99" s="32"/>
-      <c r="C99" s="104" t="s">
+      <c r="C99" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="D99" s="105"/>
-      <c r="E99" s="105"/>
-      <c r="F99" s="105"/>
-      <c r="G99" s="105"/>
-      <c r="H99" s="105"/>
-      <c r="I99" s="105"/>
-      <c r="J99" s="105"/>
-      <c r="K99" s="105"/>
+      <c r="D99" s="95"/>
+      <c r="E99" s="95"/>
+      <c r="F99" s="95"/>
+      <c r="G99" s="95"/>
+      <c r="H99" s="95"/>
+      <c r="I99" s="95"/>
+      <c r="J99" s="95"/>
+      <c r="K99" s="95"/>
       <c r="M99" s="31"/>
       <c r="N99" s="31"/>
       <c r="P99" s="31"/>
@@ -9036,17 +9033,17 @@
       <c r="B100" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C100" s="105" t="s">
+      <c r="C100" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="105"/>
-      <c r="E100" s="105"/>
-      <c r="F100" s="105"/>
-      <c r="G100" s="105"/>
-      <c r="H100" s="105"/>
-      <c r="I100" s="105"/>
-      <c r="J100" s="105"/>
-      <c r="K100" s="105"/>
+      <c r="D100" s="95"/>
+      <c r="E100" s="95"/>
+      <c r="F100" s="95"/>
+      <c r="G100" s="95"/>
+      <c r="H100" s="95"/>
+      <c r="I100" s="95"/>
+      <c r="J100" s="95"/>
+      <c r="K100" s="95"/>
       <c r="M100" s="31"/>
       <c r="N100" s="31"/>
       <c r="P100" s="31"/>
@@ -9054,17 +9051,17 @@
     <row r="101" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="30"/>
       <c r="B101" s="32"/>
-      <c r="C101" s="104" t="s">
+      <c r="C101" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="105"/>
-      <c r="E101" s="105"/>
-      <c r="F101" s="105"/>
-      <c r="G101" s="105"/>
-      <c r="H101" s="105"/>
-      <c r="I101" s="105"/>
-      <c r="J101" s="105"/>
-      <c r="K101" s="105"/>
+      <c r="D101" s="95"/>
+      <c r="E101" s="95"/>
+      <c r="F101" s="95"/>
+      <c r="G101" s="95"/>
+      <c r="H101" s="95"/>
+      <c r="I101" s="95"/>
+      <c r="J101" s="95"/>
+      <c r="K101" s="95"/>
       <c r="M101" s="31"/>
       <c r="N101" s="31"/>
       <c r="P101" s="31"/>
@@ -9074,22 +9071,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C81:K81"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="C90:K90"/>
-    <mergeCell ref="C91:K91"/>
-    <mergeCell ref="C82:K82"/>
-    <mergeCell ref="C85:K85"/>
-    <mergeCell ref="C98:K98"/>
-    <mergeCell ref="C97:K97"/>
-    <mergeCell ref="C95:K95"/>
-    <mergeCell ref="C86:K86"/>
-    <mergeCell ref="C92:K92"/>
     <mergeCell ref="C101:K101"/>
     <mergeCell ref="C100:K100"/>
     <mergeCell ref="C83:K83"/>
@@ -9100,6 +9081,22 @@
     <mergeCell ref="C96:K96"/>
     <mergeCell ref="C94:K94"/>
     <mergeCell ref="C99:K99"/>
+    <mergeCell ref="C90:K90"/>
+    <mergeCell ref="C91:K91"/>
+    <mergeCell ref="C82:K82"/>
+    <mergeCell ref="C85:K85"/>
+    <mergeCell ref="C98:K98"/>
+    <mergeCell ref="C97:K97"/>
+    <mergeCell ref="C95:K95"/>
+    <mergeCell ref="C86:K86"/>
+    <mergeCell ref="C92:K92"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C81:K81"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C101" r:id="rId1" xr:uid="{103135C5-E3C9-44D4-8173-824D09EC69E6}"/>

</xml_diff>

<commit_message>
re-run with updated costs
</commit_message>
<xml_diff>
--- a/data/school_costs/school costs.xlsx
+++ b/data/school_costs/school costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awby\github\school-cuts\data\school_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC34818-B27B-4E12-9AB2-4B789F7C43AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE875E85-A978-40B1-BCD0-F6216C9ADAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="School costs" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="216">
   <si>
     <t>Year</t>
   </si>
@@ -109,10 +109,6 @@
   </si>
   <si>
     <t>JSON</t>
-  </si>
-  <si>
-    <t>Index 
-(2021-22 = 100)</t>
   </si>
   <si>
     <t>GDP deflator</t>
@@ -819,6 +815,14 @@
   <si>
     <t>GDP deflators at market prices, and money GDP June 2022 (Quarterly National Accounts)</t>
   </si>
+  <si>
+    <t>Index 
+(2009-10 = 100)</t>
+  </si>
+  <si>
+    <t>Index 
+(2022-23 = 100)</t>
+  </si>
 </sst>
 </file>
 
@@ -831,11 +835,16 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1169,289 +1178,292 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2092,28 +2104,28 @@
                   <c:v>4.3339485860730963E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2389346354757844E-2</c:v>
+                  <c:v>5.2919083589000722E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2242939364195199E-2</c:v>
+                  <c:v>6.3083268944716456E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.3903265698847554E-2</c:v>
+                  <c:v>8.5981191011957683E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11096676891443358</c:v>
+                  <c:v>0.11381068208321372</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13790094376723294</c:v>
+                  <c:v>0.14082816010236013</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.15167340398930909</c:v>
+                  <c:v>0.15469073185586299</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16598868432091546</c:v>
+                  <c:v>0.16905092753407541</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.19279925413578464</c:v>
+                  <c:v>0.19594561767408317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3628,7 +3640,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{DD605DFA-3195-4208-A8C3-CB9564B232B3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3971,7 +3983,7 @@
   </sheetPr>
   <dimension ref="A1:Z84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3982,7 +3994,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4102,24 +4114,24 @@
     </row>
     <row r="7" spans="1:26" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="10">
         <v>0.53</v>
@@ -4134,7 +4146,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="10">
         <f>B9/SUM($B9:$C9)</f>
@@ -4147,7 +4159,7 @@
     </row>
     <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="1"/>
     </row>
@@ -4156,10 +4168,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>18</v>
@@ -4195,7 +4207,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7">
         <v>2.3E-2</v>
@@ -4227,7 +4239,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="7">
         <v>2.3E-2</v>
@@ -4273,7 +4285,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
@@ -4319,7 +4331,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -4365,7 +4377,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="7">
         <v>0.01</v>
@@ -4411,7 +4423,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="7">
         <v>0.01</v>
@@ -4495,19 +4507,19 @@
         <v>0.01</v>
       </c>
       <c r="D21" s="7">
-        <v>1.1750840465277079E-2</v>
+        <v>1.3546672214901356E-2</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" ref="E21:E29" si="4">C21*B$10+D21*C$10</f>
-        <v>1.060522880281183E-2</v>
+        <v>1.1226010148360964E-2</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="3"/>
-        <v>6.4678205376244247E-2</v>
+        <v>6.5332201961729286E-2</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="2"/>
-        <v>5.2389346354757844E-2</v>
+        <v>5.2919083589000722E-2</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -4523,19 +4535,19 @@
         <v>1.1166666666666667E-2</v>
       </c>
       <c r="D22" s="7">
-        <v>1.1916653982351866E-2</v>
+        <v>1.2937595115085632E-2</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="4"/>
-        <v>1.1425921541224515E-2</v>
+        <v>1.1778839463651002E-2</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="3"/>
-        <v>7.6843135017524933E-2</v>
+        <v>7.7880578944094392E-2</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="2"/>
-        <v>6.2242939364195199E-2</v>
+        <v>6.3083268944716456E-2</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -4551,19 +4563,19 @@
         <v>2.0750000000000001E-2</v>
       </c>
       <c r="D23" s="7">
-        <v>3.2561261836423494E-2</v>
+        <v>3.6592744449622572E-2</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="4"/>
-        <v>2.4832905326171086E-2</v>
+        <v>2.6226504254190521E-2</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="3"/>
-        <v>0.10358427864055253</v>
+        <v>0.10614961853328109</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="2"/>
-        <v>8.3903265698847554E-2</v>
+        <v>8.5981191011957683E-2</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -4578,19 +4590,19 @@
         <v>2.816666666666667E-2</v>
       </c>
       <c r="D24" s="7">
-        <v>3.4267656786153511E-2</v>
+        <v>3.6537684607055976E-2</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="4"/>
-        <v>3.0275650905501626E-2</v>
+        <v>3.1060351880628407E-2</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" ref="F24:F29" si="6">(1+F23)*(1+E24)-1</f>
-        <v>0.13699601100547354</v>
+        <v>0.1405070149175478</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" ref="G24:G29" si="7">F24*0.81</f>
-        <v>0.11096676891443358</v>
+        <v>0.11381068208321372</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -4605,19 +4617,19 @@
         <v>3.0166666666666665E-2</v>
       </c>
       <c r="D25" s="7">
-        <v>2.7501992548237819E-2</v>
+        <v>2.7502403945802945E-2</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="4"/>
-        <v>2.9245544749185087E-2</v>
+        <v>2.9245686960689084E-2</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="6"/>
-        <v>0.17024807872497894</v>
+        <v>0.17386192605229644</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="7"/>
-        <v>0.13790094376723294</v>
+        <v>0.14082816010236013</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -4632,104 +4644,104 @@
         <v>1.2916666666666667E-2</v>
       </c>
       <c r="D26" s="7">
-        <v>1.7582160023552618E-2</v>
+        <v>1.7726922568549464E-2</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="4"/>
-        <v>1.4529429802380329E-2</v>
+        <v>1.4579471175959487E-2</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" si="6"/>
-        <v>0.18725111603618405</v>
+        <v>0.19097621216773208</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="7"/>
-        <v>0.15167340398930909</v>
+        <v>0.15469073185586299</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="89">
+      <c r="B27" s="88">
         <v>3.9E-2</v>
       </c>
-      <c r="C27" s="89">
+      <c r="C27" s="88">
         <f t="shared" si="5"/>
         <v>2.2750000000000003E-2</v>
       </c>
-      <c r="D27" s="89">
+      <c r="D27" s="88">
         <v>0</v>
       </c>
-      <c r="E27" s="89">
+      <c r="E27" s="88">
         <f t="shared" si="4"/>
         <v>1.4885802469135805E-2</v>
       </c>
-      <c r="F27" s="89">
+      <c r="F27" s="88">
         <f t="shared" si="6"/>
-        <v>0.20492430163075981</v>
-      </c>
-      <c r="G27" s="89">
+        <v>0.20870484880750051</v>
+      </c>
+      <c r="G27" s="88">
         <f t="shared" si="7"/>
-        <v>0.16598868432091546</v>
+        <v>0.16905092753407541</v>
       </c>
       <c r="I27" s="80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="89">
+        <v>191</v>
+      </c>
+      <c r="B28" s="88">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C28" s="89">
+      <c r="C28" s="88">
         <f t="shared" si="5"/>
         <v>3.1416666666666669E-2</v>
       </c>
-      <c r="D28" s="89">
+      <c r="D28" s="88">
         <v>0.02</v>
       </c>
-      <c r="E28" s="89">
+      <c r="E28" s="88">
         <f t="shared" si="4"/>
         <v>2.7470164609053504E-2</v>
       </c>
-      <c r="F28" s="89">
+      <c r="F28" s="88">
         <f t="shared" si="6"/>
-        <v>0.23802377053800572</v>
-      </c>
-      <c r="G28" s="89">
+        <v>0.24190816996800391</v>
+      </c>
+      <c r="G28" s="88">
         <f t="shared" si="7"/>
-        <v>0.19279925413578464</v>
+        <v>0.19594561767408317</v>
       </c>
       <c r="I28" s="80"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="89">
+        <v>192</v>
+      </c>
+      <c r="B29" s="88">
         <v>0.02</v>
       </c>
-      <c r="C29" s="89">
+      <c r="C29" s="88">
         <f t="shared" si="5"/>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="D29" s="89">
+      <c r="D29" s="88">
         <v>0.02</v>
       </c>
-      <c r="E29" s="89">
+      <c r="E29" s="88">
         <f t="shared" si="4"/>
         <v>2.1635802469135806E-2</v>
       </c>
-      <c r="F29" s="89">
+      <c r="F29" s="88">
         <f t="shared" si="6"/>
-        <v>0.26480940828946076</v>
-      </c>
-      <c r="G29" s="89">
+        <v>0.2687778498182376</v>
+      </c>
+      <c r="G29" s="88">
         <f t="shared" si="7"/>
-        <v>0.21449562071446324</v>
+        <v>0.21771005835277246</v>
       </c>
       <c r="I29" s="80"/>
     </row>
@@ -4738,7 +4750,7 @@
     </row>
     <row r="31" spans="1:26" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B31" s="1"/>
     </row>
@@ -4747,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>16</v>
@@ -4779,7 +4791,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="12">
         <f>'30062022 deflator update'!D63/100</f>
@@ -4817,7 +4829,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="12">
         <f>'30062022 deflator update'!D64/100</f>
@@ -4855,7 +4867,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="12">
         <f>'30062022 deflator update'!D65/100</f>
@@ -4893,7 +4905,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="12">
         <f>'30062022 deflator update'!D66/100</f>
@@ -4931,7 +4943,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <f>'30062022 deflator update'!D67/100</f>
@@ -5094,10 +5106,10 @@
         <f t="shared" si="12"/>
         <v>4.8581487479021121E-2</v>
       </c>
-      <c r="F43" s="92"/>
-      <c r="G43" s="92"/>
-      <c r="H43" s="92"/>
-      <c r="I43" s="92"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="str">
@@ -5116,10 +5128,10 @@
         <f t="shared" si="12"/>
         <v>4.8054703028083873E-2</v>
       </c>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
@@ -5140,7 +5152,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B46" s="12">
         <f>'30062022 deflator update'!D76/100</f>
@@ -5157,7 +5169,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B47" s="12">
         <f>'30062022 deflator update'!D77/100</f>
@@ -5174,7 +5186,7 @@
     </row>
     <row r="49" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49" s="1"/>
     </row>
@@ -5189,7 +5201,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>9</v>
@@ -5201,7 +5213,7 @@
         <v>11</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>12</v>
@@ -5225,7 +5237,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="84"/>
       <c r="C51" s="84"/>
@@ -5263,7 +5275,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="7">
         <v>5.0000000000000001E-3</v>
@@ -5303,7 +5315,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="7">
         <v>5.0000000000000001E-3</v>
@@ -5343,7 +5355,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="7">
         <v>5.0000000000000001E-3</v>
@@ -5383,7 +5395,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="7">
         <v>5.0000000000000001E-3</v>
@@ -5474,7 +5486,7 @@
       </c>
       <c r="E57" s="7">
         <f t="shared" ref="E57:E65" si="17">G21</f>
-        <v>5.2389346354757844E-2</v>
+        <v>5.2919083589000722E-2</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7">
@@ -5487,9 +5499,9 @@
       </c>
       <c r="I57" s="7">
         <f>SUM(B57:H57)</f>
-        <v>0.10231066775326692</v>
-      </c>
-      <c r="J57" s="88"/>
+        <v>0.10284040498750979</v>
+      </c>
+      <c r="J57" s="87"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="str">
@@ -5504,7 +5516,7 @@
       </c>
       <c r="E58" s="7">
         <f t="shared" si="17"/>
-        <v>6.2242939364195199E-2</v>
+        <v>6.3083268944716456E-2</v>
       </c>
       <c r="F58" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5519,9 +5531,9 @@
       </c>
       <c r="I58" s="7">
         <f t="shared" ref="I58:I63" si="20">SUM(B58:H58)</f>
-        <v>0.12083104433332137</v>
-      </c>
-      <c r="J58" s="88"/>
+        <v>0.12167137391384263</v>
+      </c>
+      <c r="J58" s="87"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="str">
@@ -5536,7 +5548,7 @@
       </c>
       <c r="E59" s="7">
         <f t="shared" si="17"/>
-        <v>8.3903265698847554E-2</v>
+        <v>8.5981191011957683E-2</v>
       </c>
       <c r="F59" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5551,9 +5563,9 @@
       </c>
       <c r="I59" s="7">
         <f t="shared" si="20"/>
-        <v>0.14771862382165654</v>
-      </c>
-      <c r="J59" s="88"/>
+        <v>0.14979654913476667</v>
+      </c>
+      <c r="J59" s="87"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="str">
@@ -5569,7 +5581,7 @@
       </c>
       <c r="E60" s="7">
         <f t="shared" si="17"/>
-        <v>0.11096676891443358</v>
+        <v>0.11381068208321372</v>
       </c>
       <c r="F60" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5584,9 +5596,9 @@
       </c>
       <c r="I60" s="7">
         <f t="shared" si="20"/>
-        <v>0.20263784082063677</v>
-      </c>
-      <c r="J60" s="88"/>
+        <v>0.2054817539894169</v>
+      </c>
+      <c r="J60" s="87"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="str">
@@ -5606,7 +5618,7 @@
       </c>
       <c r="E61" s="7">
         <f t="shared" si="17"/>
-        <v>0.13790094376723294</v>
+        <v>0.14082816010236013</v>
       </c>
       <c r="F61" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5620,9 +5632,9 @@
       </c>
       <c r="I61" s="7">
         <f t="shared" si="20"/>
-        <v>0.2581624312462541</v>
-      </c>
-      <c r="J61" s="88"/>
+        <v>0.26108964758138126</v>
+      </c>
+      <c r="J61" s="87"/>
       <c r="K61" s="21"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
@@ -5643,7 +5655,7 @@
       </c>
       <c r="E62" s="7">
         <f t="shared" si="17"/>
-        <v>0.15167340398930909</v>
+        <v>0.15469073185586299</v>
       </c>
       <c r="F62" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5658,9 +5670,9 @@
       </c>
       <c r="I62" s="7">
         <f t="shared" si="20"/>
-        <v>0.27221810701739296</v>
-      </c>
-      <c r="J62" s="88"/>
+        <v>0.27523543488394686</v>
+      </c>
+      <c r="J62" s="87"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="str">
@@ -5680,7 +5692,7 @@
       </c>
       <c r="E63" s="7">
         <f t="shared" si="17"/>
-        <v>0.16598868432091546</v>
+        <v>0.16905092753407541</v>
       </c>
       <c r="F63" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5695,13 +5707,13 @@
       </c>
       <c r="I63" s="7">
         <f t="shared" si="20"/>
-        <v>0.30318526284927744</v>
-      </c>
-      <c r="J63" s="88"/>
+        <v>0.30624750606243739</v>
+      </c>
+      <c r="J63" s="87"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B64" s="7">
         <v>2.9000000000000001E-2</v>
@@ -5716,7 +5728,7 @@
       </c>
       <c r="E64" s="7">
         <f t="shared" si="17"/>
-        <v>0.19279925413578464</v>
+        <v>0.19594561767408317</v>
       </c>
       <c r="F64" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5731,13 +5743,13 @@
       </c>
       <c r="I64" s="7">
         <f t="shared" ref="I64:I65" si="24">SUM(B64:H64)</f>
-        <v>0.33696611091057499</v>
-      </c>
-      <c r="J64" s="88"/>
+        <v>0.34011247444887355</v>
+      </c>
+      <c r="J64" s="87"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B65" s="7">
         <v>2.9000000000000001E-2</v>
@@ -5752,7 +5764,7 @@
       </c>
       <c r="E65" s="7">
         <f t="shared" si="17"/>
-        <v>0.21449562071446324</v>
+        <v>0.21771005835277246</v>
       </c>
       <c r="F65" s="7">
         <v>3.0000000000000001E-3</v>
@@ -5767,9 +5779,9 @@
       </c>
       <c r="I65" s="7">
         <f t="shared" si="24"/>
-        <v>0.36436647607964445</v>
-      </c>
-      <c r="J65" s="88"/>
+        <v>0.36758091371795376</v>
+      </c>
+      <c r="J65" s="87"/>
     </row>
     <row r="67" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
@@ -5781,139 +5793,166 @@
         <v>0</v>
       </c>
       <c r="B68" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="81" t="s">
+      <c r="D68" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="F68" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="82"/>
+      <c r="G68" s="82"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="87">
+        <v>57</v>
+      </c>
+      <c r="B69" s="108">
         <v>100</v>
       </c>
       <c r="C69" s="18">
-        <f>B69/B$82*100</f>
-        <v>76.735060509632007</v>
-      </c>
-      <c r="E69" s="20" t="str">
-        <f t="shared" ref="E69" si="25">LEFT(A69,4)&amp;" : "&amp;C69/100&amp;","</f>
-        <v>2009 : 0.76735060509632,</v>
+        <f>$B69/$B$75*100</f>
+        <v>93.755587396072102</v>
+      </c>
+      <c r="D69" s="18">
+        <f>$B69/$B$82*100</f>
+        <v>76.555170085216687</v>
       </c>
       <c r="F69" s="20" t="str">
-        <f t="shared" ref="F69" si="26">"'"&amp;A69&amp;"' : "&amp;C69/100&amp;","</f>
-        <v>'2009-10' : 0.76735060509632,</v>
+        <f>LEFT(A69,4)&amp;" : "&amp;D69/100&amp;","</f>
+        <v>2009 : 0.765551700852167,</v>
+      </c>
+      <c r="G69" s="20" t="str">
+        <f>"'"&amp;A69&amp;"' : "&amp;D69/100&amp;","</f>
+        <v>'2009-10' : 0.765551700852167,</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="83" t="s">
-        <v>56</v>
+      <c r="A70" s="109" t="s">
+        <v>55</v>
       </c>
       <c r="B70" s="18">
-        <f t="shared" ref="B70:B75" si="27">100+100*I51</f>
+        <f>100+100*I51</f>
         <v>101.53584261299153</v>
       </c>
       <c r="C70" s="18">
-        <f t="shared" ref="C70:C84" si="28">B70/B$82*100</f>
-        <v>77.913590268043777</v>
-      </c>
-      <c r="E70" s="20" t="str">
-        <f t="shared" ref="E70:E74" si="29">LEFT(A70,4)&amp;" : "&amp;C70/100&amp;","</f>
-        <v>2010 : 0.779135902680438,</v>
+        <f t="shared" ref="C70:C84" si="25">$B70/$B$75*100</f>
+        <v>95.195525659361493</v>
+      </c>
+      <c r="D70" s="18">
+        <f t="shared" ref="C70:D84" si="26">$B70/$B$82*100</f>
+        <v>77.730937009833582</v>
       </c>
       <c r="F70" s="20" t="str">
-        <f t="shared" ref="F70:F74" si="30">"'"&amp;A70&amp;"' : "&amp;C70/100&amp;","</f>
-        <v>'2010-11' : 0.779135902680438,</v>
+        <f>LEFT(A70,4)&amp;" : "&amp;D70/100&amp;","</f>
+        <v>2010 : 0.777309370098336,</v>
+      </c>
+      <c r="G70" s="20" t="str">
+        <f>"'"&amp;A70&amp;"' : "&amp;D70/100&amp;","</f>
+        <v>'2010-11' : 0.777309370098336,</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="83" t="s">
-        <v>54</v>
+      <c r="A71" s="109" t="s">
+        <v>53</v>
       </c>
       <c r="B71" s="18">
-        <f t="shared" si="27"/>
+        <f>100+100*I52</f>
         <v>102.84318640271631</v>
       </c>
       <c r="C71" s="18">
-        <f t="shared" si="28"/>
-        <v>78.916781316158009</v>
-      </c>
-      <c r="E71" s="20" t="str">
-        <f t="shared" si="29"/>
-        <v>2011 : 0.78916781316158,</v>
+        <f t="shared" si="25"/>
+        <v>96.421233508704034</v>
+      </c>
+      <c r="D71" s="18">
+        <f t="shared" si="26"/>
+        <v>78.731776271655903</v>
       </c>
       <c r="F71" s="20" t="str">
-        <f t="shared" si="30"/>
-        <v>'2011-12' : 0.78916781316158,</v>
+        <f>LEFT(A71,4)&amp;" : "&amp;D71/100&amp;","</f>
+        <v>2011 : 0.787317762716559,</v>
+      </c>
+      <c r="G71" s="20" t="str">
+        <f>"'"&amp;A71&amp;"' : "&amp;D71/100&amp;","</f>
+        <v>'2011-12' : 0.787317762716559,</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="83" t="s">
-        <v>53</v>
+      <c r="A72" s="109" t="s">
+        <v>52</v>
       </c>
       <c r="B72" s="18">
-        <f t="shared" si="27"/>
+        <f>100+100*I53</f>
         <v>103.2385748729467</v>
       </c>
       <c r="C72" s="18">
-        <f t="shared" si="28"/>
-        <v>79.220182898037393</v>
-      </c>
-      <c r="E72" s="20" t="str">
-        <f t="shared" si="29"/>
-        <v>2012 : 0.792201828980374,</v>
+        <f t="shared" si="25"/>
+        <v>96.791932291464875</v>
+      </c>
+      <c r="D72" s="18">
+        <f t="shared" si="26"/>
+        <v>79.03446658753812</v>
       </c>
       <c r="F72" s="20" t="str">
-        <f t="shared" si="30"/>
-        <v>'2012-13' : 0.792201828980374,</v>
+        <f>LEFT(A72,4)&amp;" : "&amp;D72/100&amp;","</f>
+        <v>2012 : 0.790344665875381,</v>
+      </c>
+      <c r="G72" s="20" t="str">
+        <f>"'"&amp;A72&amp;"' : "&amp;D72/100&amp;","</f>
+        <v>'2012-13' : 0.790344665875381,</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="83" t="s">
-        <v>52</v>
+      <c r="A73" s="109" t="s">
+        <v>51</v>
       </c>
       <c r="B73" s="18">
-        <f t="shared" si="27"/>
+        <f>100+100*I54</f>
         <v>104.29856436651735</v>
       </c>
       <c r="C73" s="18">
-        <f t="shared" si="28"/>
-        <v>80.033566477324584</v>
-      </c>
-      <c r="E73" s="20" t="str">
-        <f t="shared" si="29"/>
-        <v>2013 : 0.800335664773246,</v>
+        <f t="shared" si="25"/>
+        <v>97.785731667498681</v>
+      </c>
+      <c r="D73" s="18">
+        <f t="shared" si="26"/>
+        <v>79.845943347226552</v>
       </c>
       <c r="F73" s="20" t="str">
-        <f t="shared" si="30"/>
-        <v>'2013-14' : 0.800335664773246,</v>
+        <f>LEFT(A73,4)&amp;" : "&amp;D73/100&amp;","</f>
+        <v>2013 : 0.798459433472266,</v>
+      </c>
+      <c r="G73" s="20" t="str">
+        <f>"'"&amp;A73&amp;"' : "&amp;D73/100&amp;","</f>
+        <v>'2013-14' : 0.798459433472266,</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="83" t="s">
-        <v>51</v>
+      <c r="A74" s="109" t="s">
+        <v>50</v>
       </c>
       <c r="B74" s="18">
-        <f t="shared" si="27"/>
+        <f>100+100*I55</f>
         <v>105.97717962588322</v>
       </c>
       <c r="C74" s="18">
-        <f t="shared" si="28"/>
-        <v>81.32165291232289</v>
-      </c>
-      <c r="E74" s="20" t="str">
-        <f t="shared" si="29"/>
-        <v>2014 : 0.813216529123229,</v>
+        <f t="shared" si="25"/>
+        <v>99.359527264037268</v>
+      </c>
+      <c r="D74" s="18">
+        <f t="shared" si="26"/>
+        <v>81.131010114110495</v>
       </c>
       <c r="F74" s="20" t="str">
-        <f t="shared" si="30"/>
-        <v>'2014-15' : 0.813216529123229,</v>
+        <f>LEFT(A74,4)&amp;" : "&amp;D74/100&amp;","</f>
+        <v>2014 : 0.811310101141105,</v>
+      </c>
+      <c r="G74" s="20" t="str">
+        <f>"'"&amp;A74&amp;"' : "&amp;D74/100&amp;","</f>
+        <v>'2014-15' : 0.811310101141105,</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -5921,216 +5960,256 @@
         <v>1</v>
       </c>
       <c r="B75" s="18">
-        <f t="shared" si="27"/>
+        <f>100+100*I56</f>
         <v>106.66030983044058</v>
       </c>
       <c r="C75" s="18">
-        <f t="shared" si="28"/>
-        <v>81.845853288149556</v>
-      </c>
-      <c r="E75" s="20" t="str">
-        <f t="shared" ref="E75:E84" si="31">LEFT(A75,4)&amp;" : "&amp;C75/100&amp;","</f>
-        <v>2015 : 0.818458532881496,</v>
+        <f t="shared" si="25"/>
+        <v>100</v>
+      </c>
+      <c r="D75" s="18">
+        <f t="shared" si="26"/>
+        <v>81.653981604112886</v>
       </c>
       <c r="F75" s="20" t="str">
-        <f>"'"&amp;A75&amp;"' : "&amp;C75/100&amp;","</f>
-        <v>'2015-16' : 0.818458532881496,</v>
+        <f>LEFT(A75,4)&amp;" : "&amp;D75/100&amp;","</f>
+        <v>2015 : 0.816539816041129,</v>
+      </c>
+      <c r="G75" s="20" t="str">
+        <f>"'"&amp;A75&amp;"' : "&amp;D75/100&amp;","</f>
+        <v>'2015-16' : 0.816539816041129,</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="str">
-        <f t="shared" ref="A76:A82" si="32">A57</f>
+        <f t="shared" ref="A76:A82" si="27">A57</f>
         <v>2016-17</v>
       </c>
       <c r="B76" s="18">
-        <f t="shared" ref="B76:B84" si="33">100+100*I57</f>
-        <v>110.2310667753267</v>
+        <f>100+100*I57</f>
+        <v>110.28404049875098</v>
       </c>
       <c r="C76" s="18">
-        <f t="shared" si="28"/>
-        <v>84.585875790459809</v>
-      </c>
-      <c r="E76" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2016 : 0.845858757904598,</v>
+        <f t="shared" si="25"/>
+        <v>103.39744997372603</v>
+      </c>
+      <c r="D76" s="18">
+        <f t="shared" si="26"/>
+        <v>84.42813478066806</v>
       </c>
       <c r="F76" s="20" t="str">
-        <f t="shared" ref="F76:F84" si="34">"'"&amp;A76&amp;"' : "&amp;C76/100&amp;","</f>
-        <v>'2016-17' : 0.845858757904598,</v>
+        <f>LEFT(A76,4)&amp;" : "&amp;D76/100&amp;","</f>
+        <v>2016 : 0.844281347806681,</v>
+      </c>
+      <c r="G76" s="20" t="str">
+        <f>"'"&amp;A76&amp;"' : "&amp;D76/100&amp;","</f>
+        <v>'2016-17' : 0.844281347806681,</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2017-18</v>
       </c>
       <c r="B77" s="18">
-        <f t="shared" si="33"/>
-        <v>112.08310443333214</v>
+        <f>100+100*I58</f>
+        <v>112.16713739138426</v>
       </c>
       <c r="C77" s="18">
-        <f t="shared" si="28"/>
-        <v>86.007038007991454</v>
-      </c>
-      <c r="E77" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2017 : 0.860070380079915,</v>
+        <f t="shared" si="25"/>
+        <v>105.16295852665154</v>
+      </c>
+      <c r="D77" s="18">
+        <f t="shared" si="26"/>
+        <v>85.869742809692895</v>
       </c>
       <c r="F77" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2017-18' : 0.860070380079915,</v>
+        <f>LEFT(A77,4)&amp;" : "&amp;D77/100&amp;","</f>
+        <v>2017 : 0.858697428096929,</v>
+      </c>
+      <c r="G77" s="20" t="str">
+        <f>"'"&amp;A77&amp;"' : "&amp;D77/100&amp;","</f>
+        <v>'2017-18' : 0.858697428096929,</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2018-19</v>
       </c>
       <c r="B78" s="18">
-        <f t="shared" si="33"/>
-        <v>114.77186238216565</v>
+        <f>100+100*I59</f>
+        <v>114.97965491347667</v>
       </c>
       <c r="C78" s="18">
-        <f t="shared" si="28"/>
-        <v>88.070258046986396</v>
-      </c>
-      <c r="E78" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2018 : 0.880702580469864,</v>
+        <f t="shared" si="25"/>
+        <v>107.79985085010672</v>
+      </c>
+      <c r="D78" s="18">
+        <f t="shared" si="26"/>
+        <v>88.022870382407262</v>
       </c>
       <c r="F78" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2018-19' : 0.880702580469864,</v>
+        <f>LEFT(A78,4)&amp;" : "&amp;D78/100&amp;","</f>
+        <v>2018 : 0.880228703824073,</v>
+      </c>
+      <c r="G78" s="20" t="str">
+        <f>"'"&amp;A78&amp;"' : "&amp;D78/100&amp;","</f>
+        <v>'2018-19' : 0.880228703824073,</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2019-20</v>
       </c>
       <c r="B79" s="18">
-        <f t="shared" si="33"/>
-        <v>120.26378408206368</v>
+        <f>100+100*I60</f>
+        <v>120.54817539894169</v>
       </c>
       <c r="C79" s="18">
-        <f t="shared" si="28"/>
-        <v>92.284487486544748</v>
-      </c>
-      <c r="E79" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2019 : 0.922844874865448,</v>
+        <f t="shared" si="25"/>
+        <v>113.02064994052508</v>
+      </c>
+      <c r="D79" s="18">
+        <f t="shared" si="26"/>
+        <v>92.285860711285153</v>
       </c>
       <c r="F79" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2019-20' : 0.922844874865448,</v>
+        <f>LEFT(A79,4)&amp;" : "&amp;D79/100&amp;","</f>
+        <v>2019 : 0.922858607112852,</v>
+      </c>
+      <c r="G79" s="20" t="str">
+        <f>"'"&amp;A79&amp;"' : "&amp;D79/100&amp;","</f>
+        <v>'2019-20' : 0.922858607112852,</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2020-21</v>
       </c>
       <c r="B80" s="18">
-        <f t="shared" si="33"/>
-        <v>125.8162431246254</v>
+        <f>100+100*I61</f>
+        <v>126.10896475813813</v>
       </c>
       <c r="C80" s="18">
-        <f t="shared" si="28"/>
-        <v>96.54517029262702</v>
-      </c>
-      <c r="E80" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2020 : 0.96545170292627,</v>
+        <f t="shared" si="25"/>
+        <v>118.23420066809796</v>
+      </c>
+      <c r="D80" s="18">
+        <f t="shared" si="26"/>
+        <v>96.542932463298598</v>
       </c>
       <c r="F80" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2020-21' : 0.96545170292627,</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f>LEFT(A80,4)&amp;" : "&amp;D80/100&amp;","</f>
+        <v>2020 : 0.965429324632986,</v>
+      </c>
+      <c r="G80" s="20" t="str">
+        <f>"'"&amp;A80&amp;"' : "&amp;D80/100&amp;","</f>
+        <v>'2020-21' : 0.965429324632986,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2021-22</v>
       </c>
       <c r="B81" s="18">
-        <f t="shared" si="33"/>
-        <v>127.2218107017393</v>
+        <f>100+100*I62</f>
+        <v>127.52354348839469</v>
       </c>
       <c r="C81" s="18">
-        <f t="shared" si="28"/>
-        <v>97.623733423429144</v>
-      </c>
-      <c r="E81" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2021 : 0.976237334234291,</v>
+        <f t="shared" si="25"/>
+        <v>119.56044726582991</v>
+      </c>
+      <c r="D81" s="18">
+        <f t="shared" si="26"/>
+        <v>97.625865616235814</v>
       </c>
       <c r="F81" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2021-22' : 0.976237334234291,</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f>LEFT(A81,4)&amp;" : "&amp;D81/100&amp;","</f>
+        <v>2021 : 0.976258656162358,</v>
+      </c>
+      <c r="G81" s="20" t="str">
+        <f>"'"&amp;A81&amp;"' : "&amp;D81/100&amp;","</f>
+        <v>'2021-22' : 0.976258656162358,</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>2022-23</v>
       </c>
       <c r="B82" s="18">
-        <f t="shared" si="33"/>
-        <v>130.31852628492774</v>
+        <f>100+100*I63</f>
+        <v>130.62475060624374</v>
       </c>
       <c r="C82" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
+        <v>122.46800221553806</v>
+      </c>
+      <c r="D82" s="18">
+        <f t="shared" si="26"/>
         <v>100</v>
       </c>
-      <c r="E82" s="20" t="str">
-        <f t="shared" si="31"/>
+      <c r="F82" s="20" t="str">
+        <f>LEFT(A82,4)&amp;" : "&amp;D82/100&amp;","</f>
         <v>2022 : 1,</v>
       </c>
-      <c r="F82" s="20" t="str">
-        <f t="shared" si="34"/>
+      <c r="G82" s="20" t="str">
+        <f>"'"&amp;A82&amp;"' : "&amp;D82/100&amp;","</f>
         <v>'2022-23' : 1,</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" s="18">
+        <f>100+100*I64</f>
+        <v>134.01124744488735</v>
+      </c>
+      <c r="C83" s="18">
+        <f t="shared" si="25"/>
+        <v>125.64303221875778</v>
+      </c>
+      <c r="D83" s="18">
+        <f t="shared" si="26"/>
+        <v>102.5925384147541</v>
+      </c>
+      <c r="F83" s="20" t="str">
+        <f>LEFT(A83,4)&amp;" : "&amp;D83/100&amp;","</f>
+        <v>2023 : 1.02592538414754,</v>
+      </c>
+      <c r="G83" s="20" t="str">
+        <f>"'"&amp;A83&amp;"' : "&amp;D83/100&amp;","</f>
+        <v>'2023-24' : 1.02592538414754,</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B83" s="18">
-        <f t="shared" si="33"/>
-        <v>133.69661109105749</v>
-      </c>
-      <c r="C83" s="18">
-        <f t="shared" si="28"/>
-        <v>102.59217542005035</v>
-      </c>
-      <c r="E83" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2023 : 1.0259217542005,</v>
-      </c>
-      <c r="F83" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2023-24' : 1.0259217542005,</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="B84" s="18">
-        <f t="shared" si="33"/>
-        <v>136.43664760796446</v>
+        <f>100+100*I65</f>
+        <v>136.75809137179539</v>
       </c>
       <c r="C84" s="18">
-        <f t="shared" si="28"/>
-        <v>104.69474409928492</v>
-      </c>
-      <c r="E84" s="20" t="str">
-        <f t="shared" si="31"/>
-        <v>2024 : 1.04694744099285,</v>
+        <f t="shared" si="25"/>
+        <v>128.21835187728377</v>
+      </c>
+      <c r="D84" s="18">
+        <f t="shared" si="26"/>
+        <v>104.69538945497401</v>
       </c>
       <c r="F84" s="20" t="str">
-        <f t="shared" si="34"/>
-        <v>'2024-25' : 1.04694744099285,</v>
+        <f>LEFT(A84,4)&amp;" : "&amp;D84/100&amp;","</f>
+        <v>2024 : 1.04695389454974,</v>
+      </c>
+      <c r="G84" s="20" t="str">
+        <f>"'"&amp;A84&amp;"' : "&amp;D84/100&amp;","</f>
+        <v>'2024-25' : 1.04695389454974,</v>
       </c>
     </row>
   </sheetData>
@@ -6155,32 +6234,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -6223,134 +6302,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="91"/>
+      <c r="A1" s="90"/>
       <c r="B1" s="77" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="76"/>
       <c r="D1" s="75"/>
       <c r="E1" s="74"/>
       <c r="F1" s="74"/>
-      <c r="G1" s="91"/>
+      <c r="G1" s="90"/>
       <c r="I1" s="25"/>
       <c r="J1" s="24"/>
       <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:13" s="26" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="91"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="77"/>
       <c r="C2" s="76"/>
       <c r="D2" s="75"/>
       <c r="E2" s="74"/>
       <c r="F2" s="74"/>
-      <c r="G2" s="91"/>
+      <c r="G2" s="90"/>
       <c r="I2" s="25"/>
       <c r="J2" s="24"/>
       <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
-      <c r="B3" s="93" t="s">
-        <v>213</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
+      <c r="B3" s="92" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
-      <c r="B4" s="94" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
+      <c r="B4" s="93" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="97"/>
+    </row>
+    <row r="6" spans="1:13" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="90"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="99"/>
+      <c r="E6" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="70"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" s="101"/>
+      <c r="K6" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="96" t="s">
+    </row>
+    <row r="7" spans="1:13" s="36" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89"/>
+      <c r="B7" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="62" t="s">
         <v>170</v>
-      </c>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="98"/>
-    </row>
-    <row r="6" spans="1:13" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="91"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="99" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="101" t="s">
-        <v>175</v>
-      </c>
-      <c r="J6" s="102"/>
-      <c r="K6" s="68" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="36" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="65" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="F7" s="62" t="s">
-        <v>171</v>
       </c>
       <c r="G7" s="66"/>
       <c r="H7" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I7" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J7" s="63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K7" s="62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="59">
         <v>3.7045611222589594</v>
@@ -6364,7 +6443,7 @@
       </c>
       <c r="G8" s="56"/>
       <c r="H8" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I8" s="59">
         <v>3.6756000000000002</v>
@@ -6377,9 +6456,9 @@
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" s="59">
         <v>3.9365531616644041</v>
@@ -6395,7 +6474,7 @@
       </c>
       <c r="G9" s="56"/>
       <c r="H9" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I9" s="59">
         <v>3.9304000000000001</v>
@@ -6410,9 +6489,9 @@
       <c r="M9" s="34"/>
     </row>
     <row r="10" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="59">
         <v>4.1179248052049431</v>
@@ -6428,7 +6507,7 @@
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I10" s="59">
         <v>4.0877999999999997</v>
@@ -6443,9 +6522,9 @@
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" s="59">
         <v>4.2174967729120585</v>
@@ -6461,7 +6540,7 @@
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11" s="59">
         <v>4.2374000000000001</v>
@@ -6476,9 +6555,9 @@
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="59">
         <v>4.2382231088419395</v>
@@ -6494,7 +6573,7 @@
       </c>
       <c r="G12" s="56"/>
       <c r="H12" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I12" s="59">
         <v>4.2682000000000002</v>
@@ -6509,9 +6588,9 @@
       <c r="M12" s="34"/>
     </row>
     <row r="13" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="90"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="59">
         <v>4.3246286935304816</v>
@@ -6527,7 +6606,7 @@
       </c>
       <c r="G13" s="56"/>
       <c r="H13" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I13" s="59">
         <v>4.3125</v>
@@ -6542,9 +6621,9 @@
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="59">
         <v>4.4827224339263747</v>
@@ -6560,7 +6639,7 @@
       </c>
       <c r="G14" s="56"/>
       <c r="H14" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I14" s="59">
         <v>4.4759000000000002</v>
@@ -6575,9 +6654,9 @@
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="90"/>
+      <c r="A15" s="89"/>
       <c r="B15" s="61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="59">
         <v>4.6236486806230772</v>
@@ -6593,7 +6672,7 @@
       </c>
       <c r="G15" s="56"/>
       <c r="H15" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I15" s="59">
         <v>4.6372</v>
@@ -6608,9 +6687,9 @@
       <c r="M15" s="34"/>
     </row>
     <row r="16" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
+      <c r="A16" s="89"/>
       <c r="B16" s="61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="59">
         <v>4.7002172191387466</v>
@@ -6626,7 +6705,7 @@
       </c>
       <c r="G16" s="56"/>
       <c r="H16" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I16" s="59">
         <v>4.7049000000000003</v>
@@ -6643,7 +6722,7 @@
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
       <c r="B17" s="54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="50">
         <v>4.9217836703036948</v>
@@ -6659,7 +6738,7 @@
       </c>
       <c r="G17" s="56"/>
       <c r="H17" s="51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I17" s="50">
         <v>4.8733000000000004</v>
@@ -6676,7 +6755,7 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="30"/>
       <c r="B18" s="54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="39">
         <v>5.1869568542678666</v>
@@ -6692,7 +6771,7 @@
       </c>
       <c r="G18" s="56"/>
       <c r="H18" s="51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I18" s="50">
         <v>5.1630000000000003</v>
@@ -6709,7 +6788,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="30"/>
       <c r="B19" s="54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="39">
         <v>5.4516809692703152</v>
@@ -6725,7 +6804,7 @@
       </c>
       <c r="G19" s="56"/>
       <c r="H19" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I19" s="50">
         <v>5.4386999999999999</v>
@@ -6742,7 +6821,7 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="30"/>
       <c r="B20" s="54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="39">
         <v>5.6005751573256681</v>
@@ -6758,7 +6837,7 @@
       </c>
       <c r="G20" s="56"/>
       <c r="H20" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I20" s="50">
         <v>5.5991</v>
@@ -6775,7 +6854,7 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
       <c r="B21" s="54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C21" s="39">
         <v>5.8936472282715364</v>
@@ -6791,7 +6870,7 @@
       </c>
       <c r="G21" s="56"/>
       <c r="H21" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I21" s="50">
         <v>5.8341000000000003</v>
@@ -6808,7 +6887,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="30"/>
       <c r="B22" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" s="39">
         <v>6.300322817649489</v>
@@ -6824,7 +6903,7 @@
       </c>
       <c r="G22" s="56"/>
       <c r="H22" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I22" s="50">
         <v>6.2207999999999997</v>
@@ -6841,7 +6920,7 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
       <c r="B23" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="39">
         <v>6.9219322171084556</v>
@@ -6857,7 +6936,7 @@
       </c>
       <c r="G23" s="56"/>
       <c r="H23" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I23" s="50">
         <v>6.8186999999999998</v>
@@ -6874,7 +6953,7 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="30"/>
       <c r="B24" s="54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="39">
         <v>7.4450041091297283</v>
@@ -6890,7 +6969,7 @@
       </c>
       <c r="G24" s="56"/>
       <c r="H24" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="50">
         <v>7.3834999999999997</v>
@@ -6907,7 +6986,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="30"/>
       <c r="B25" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" s="39">
         <v>8.0773133808835773</v>
@@ -6923,7 +7002,7 @@
       </c>
       <c r="G25" s="56"/>
       <c r="H25" s="51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I25" s="50">
         <v>7.9412000000000003</v>
@@ -6940,7 +7019,7 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="39">
         <v>8.7876926700969751</v>
@@ -6956,7 +7035,7 @@
       </c>
       <c r="G26" s="56"/>
       <c r="H26" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I26" s="50">
         <v>8.6450999999999993</v>
@@ -6973,7 +7052,7 @@
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
       <c r="B27" s="54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" s="39">
         <v>10.571065614547681</v>
@@ -6989,7 +7068,7 @@
       </c>
       <c r="G27" s="56"/>
       <c r="H27" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I27" s="50">
         <v>10.041600000000001</v>
@@ -7006,7 +7085,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="39">
         <v>13.161147299988325</v>
@@ -7022,7 +7101,7 @@
       </c>
       <c r="G28" s="56"/>
       <c r="H28" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I28" s="50">
         <v>12.6676</v>
@@ -7039,7 +7118,7 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
       <c r="B29" s="54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="39">
         <v>14.993126263247214</v>
@@ -7055,7 +7134,7 @@
       </c>
       <c r="G29" s="56"/>
       <c r="H29" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I29" s="50">
         <v>14.6271</v>
@@ -7072,7 +7151,7 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="39">
         <v>17.056458793937885</v>
@@ -7088,7 +7167,7 @@
       </c>
       <c r="G30" s="56"/>
       <c r="H30" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I30" s="50">
         <v>16.655200000000001</v>
@@ -7105,7 +7184,7 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
       <c r="B31" s="54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C31" s="39">
         <v>18.976731396128805</v>
@@ -7121,7 +7200,7 @@
       </c>
       <c r="G31" s="56"/>
       <c r="H31" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I31" s="50">
         <v>18.622199999999999</v>
@@ -7138,7 +7217,7 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
       <c r="B32" s="54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="39">
         <v>22.176541184707769</v>
@@ -7154,7 +7233,7 @@
       </c>
       <c r="G32" s="56"/>
       <c r="H32" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I32" s="50">
         <v>21.311900000000001</v>
@@ -7171,7 +7250,7 @@
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
       <c r="B33" s="54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" s="39">
         <v>26.416564539589451</v>
@@ -7187,7 +7266,7 @@
       </c>
       <c r="G33" s="56"/>
       <c r="H33" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I33" s="50">
         <v>25.6187</v>
@@ -7204,7 +7283,7 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="39">
         <v>29.199183292472974</v>
@@ -7220,7 +7299,7 @@
       </c>
       <c r="G34" s="56"/>
       <c r="H34" s="51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I34" s="50">
         <v>28.776700000000002</v>
@@ -7237,7 +7316,7 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="B35" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="39">
         <v>31.347210200962628</v>
@@ -7253,7 +7332,7 @@
       </c>
       <c r="G35" s="56"/>
       <c r="H35" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I35" s="50">
         <v>31.080400000000001</v>
@@ -7270,7 +7349,7 @@
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
       <c r="B36" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" s="39">
         <v>32.844118969839165</v>
@@ -7286,7 +7365,7 @@
       </c>
       <c r="G36" s="56"/>
       <c r="H36" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I36" s="50">
         <v>32.802500000000002</v>
@@ -7303,7 +7382,7 @@
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="30"/>
       <c r="B37" s="54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="39">
         <v>34.713487840076588</v>
@@ -7319,7 +7398,7 @@
       </c>
       <c r="G37" s="56"/>
       <c r="H37" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I37" s="50">
         <v>34.515099999999997</v>
@@ -7336,7 +7415,7 @@
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
       <c r="B38" s="54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="39">
         <v>36.645771646174254</v>
@@ -7352,7 +7431,7 @@
       </c>
       <c r="G38" s="56"/>
       <c r="H38" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I38" s="50">
         <v>36.374499999999998</v>
@@ -7369,7 +7448,7 @@
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="39">
         <v>38.170840784114105</v>
@@ -7385,7 +7464,7 @@
       </c>
       <c r="G39" s="56"/>
       <c r="H39" s="51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I39" s="50">
         <v>38.005400000000002</v>
@@ -7402,7 +7481,7 @@
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="30"/>
       <c r="B40" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" s="39">
         <v>40.349128210015209</v>
@@ -7418,7 +7497,7 @@
       </c>
       <c r="G40" s="56"/>
       <c r="H40" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I40" s="50">
         <v>40.080800000000004</v>
@@ -7435,7 +7514,7 @@
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="39">
         <v>43.058589614100562</v>
@@ -7451,7 +7530,7 @@
       </c>
       <c r="G41" s="56"/>
       <c r="H41" s="51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I41" s="50">
         <v>42.527999999999999</v>
@@ -7468,7 +7547,7 @@
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="30"/>
       <c r="B42" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42" s="39">
         <v>46.466236466755198</v>
@@ -7484,7 +7563,7 @@
       </c>
       <c r="G42" s="56"/>
       <c r="H42" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I42" s="50">
         <v>45.938299999999998</v>
@@ -7501,7 +7580,7 @@
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" s="39">
         <v>50.36109597743836</v>
@@ -7517,7 +7596,7 @@
       </c>
       <c r="G43" s="56"/>
       <c r="H43" s="51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I43" s="50">
         <v>49.719499999999996</v>
@@ -7534,7 +7613,7 @@
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="39">
         <v>53.354313520096504</v>
@@ -7550,7 +7629,7 @@
       </c>
       <c r="G44" s="56"/>
       <c r="H44" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I44" s="50">
         <v>53.087299999999999</v>
@@ -7567,7 +7646,7 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
       <c r="B45" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" s="39">
         <v>54.816702243733658</v>
@@ -7583,7 +7662,7 @@
       </c>
       <c r="G45" s="56"/>
       <c r="H45" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I45" s="50">
         <v>54.827399999999997</v>
@@ -7600,7 +7679,7 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
       <c r="B46" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="39">
         <v>56.247736656785619</v>
@@ -7616,7 +7695,7 @@
       </c>
       <c r="G46" s="56"/>
       <c r="H46" s="51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I46" s="50">
         <v>56.400599999999997</v>
@@ -7633,7 +7712,7 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C47" s="39">
         <v>57.042462981733401</v>
@@ -7649,7 +7728,7 @@
       </c>
       <c r="G47" s="56"/>
       <c r="H47" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I47" s="50">
         <v>57.232700000000001</v>
@@ -7666,7 +7745,7 @@
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
       <c r="B48" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="39">
         <v>58.800515418172594</v>
@@ -7682,7 +7761,7 @@
       </c>
       <c r="G48" s="56"/>
       <c r="H48" s="51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I48" s="50">
         <v>58.681899999999999</v>
@@ -7699,7 +7778,7 @@
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
       <c r="B49" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="39">
         <v>60.899493228798079</v>
@@ -7715,7 +7794,7 @@
       </c>
       <c r="G49" s="56"/>
       <c r="H49" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I49" s="50">
         <v>61.180500000000002</v>
@@ -7732,7 +7811,7 @@
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="39">
         <v>60.641990633513274</v>
@@ -7748,7 +7827,7 @@
       </c>
       <c r="G50" s="56"/>
       <c r="H50" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I50" s="50">
         <v>60.972099999999998</v>
@@ -7765,7 +7844,7 @@
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
       <c r="B51" s="54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="39">
         <v>62.027034418802685</v>
@@ -7781,7 +7860,7 @@
       </c>
       <c r="G51" s="56"/>
       <c r="H51" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I51" s="50">
         <v>61.940800000000003</v>
@@ -7798,7 +7877,7 @@
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="39">
         <v>62.379100293327753</v>
@@ -7814,7 +7893,7 @@
       </c>
       <c r="G52" s="56"/>
       <c r="H52" s="51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I52" s="50">
         <v>62.780200000000001</v>
@@ -7831,7 +7910,7 @@
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
       <c r="B53" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" s="39">
         <v>63.618555063360844</v>
@@ -7847,7 +7926,7 @@
       </c>
       <c r="G53" s="56"/>
       <c r="H53" s="51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I53" s="50">
         <v>63.837400000000002</v>
@@ -7864,7 +7943,7 @@
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" s="39">
         <v>64.946690444991134</v>
@@ -7880,7 +7959,7 @@
       </c>
       <c r="G54" s="56"/>
       <c r="H54" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I54" s="50">
         <v>65.019000000000005</v>
@@ -7897,7 +7976,7 @@
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="30"/>
       <c r="B55" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="39">
         <v>66.323221507673139</v>
@@ -7913,7 +7992,7 @@
       </c>
       <c r="G55" s="56"/>
       <c r="H55" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I55" s="50">
         <v>66.358500000000006</v>
@@ -7930,7 +8009,7 @@
     <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="39">
         <v>68.00985451553251</v>
@@ -7946,7 +8025,7 @@
       </c>
       <c r="G56" s="56"/>
       <c r="H56" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I56" s="50">
         <v>68.173599999999993</v>
@@ -7963,7 +8042,7 @@
     <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
       <c r="B57" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="39">
         <v>70.028722704648928</v>
@@ -7979,7 +8058,7 @@
       </c>
       <c r="G57" s="56"/>
       <c r="H57" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I57" s="50">
         <v>69.927999999999997</v>
@@ -7996,7 +8075,7 @@
     <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
       <c r="B58" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="39">
         <v>72.104353359893793</v>
@@ -8012,7 +8091,7 @@
       </c>
       <c r="G58" s="56"/>
       <c r="H58" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I58" s="50">
         <v>72.117800000000003</v>
@@ -8030,7 +8109,7 @@
     <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
       <c r="B59" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="39">
         <v>74.242876785182261</v>
@@ -8046,7 +8125,7 @@
       </c>
       <c r="G59" s="56"/>
       <c r="H59" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I59" s="50">
         <v>74.1755</v>
@@ -8060,14 +8139,14 @@
       <c r="L59" s="56"/>
       <c r="M59" s="34"/>
       <c r="O59" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R59" s="27"/>
     </row>
     <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
       <c r="B60" s="54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" s="39">
         <v>76.318042080173214</v>
@@ -8083,7 +8162,7 @@
       </c>
       <c r="G60" s="56"/>
       <c r="H60" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I60" s="50">
         <v>76.249499999999998</v>
@@ -8101,7 +8180,7 @@
     <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
       <c r="B61" s="54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="39">
         <v>78.578857661075645</v>
@@ -8117,7 +8196,7 @@
       </c>
       <c r="G61" s="56"/>
       <c r="H61" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I61" s="50">
         <v>78.726799999999997</v>
@@ -8135,7 +8214,7 @@
     <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="B62" s="54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" s="39">
         <v>79.813588046435342</v>
@@ -8151,7 +8230,7 @@
       </c>
       <c r="G62" s="56"/>
       <c r="H62" s="51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I62" s="50">
         <v>80.066000000000003</v>
@@ -8168,7 +8247,7 @@
     <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" s="39">
         <v>81.14455361427018</v>
@@ -8184,7 +8263,7 @@
       </c>
       <c r="G63" s="56"/>
       <c r="H63" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I63" s="50">
         <v>81.165700000000001</v>
@@ -8201,7 +8280,7 @@
     <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
       <c r="B64" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C64" s="39">
         <v>82.370252107272321</v>
@@ -8234,7 +8313,7 @@
     <row r="65" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C65" s="39">
         <v>84.031166448392241</v>
@@ -8267,7 +8346,7 @@
     <row r="66" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
       <c r="B66" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66" s="39">
         <v>85.955960259776646</v>
@@ -8300,7 +8379,7 @@
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C67" s="39">
         <v>86.94623130094223</v>
@@ -8553,10 +8632,10 @@
     <row r="75" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
       <c r="B75" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C75" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D75" s="49">
         <v>4.0544779739719816</v>
@@ -8568,10 +8647,10 @@
         <v>2512583</v>
       </c>
       <c r="H75" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I75" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J75" s="49">
         <v>2.8492930312000952</v>
@@ -8583,10 +8662,10 @@
     <row r="76" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="30"/>
       <c r="B76" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C76" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D76" s="49">
         <v>2.4102219173580908</v>
@@ -8598,10 +8677,10 @@
         <v>2622335</v>
       </c>
       <c r="H76" s="51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I76" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J76" s="49">
         <v>3.143440902459993</v>
@@ -8613,10 +8692,10 @@
     <row r="77" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
       <c r="B77" s="54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C77" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D77" s="49">
         <v>1.8543270561598879</v>
@@ -8628,10 +8707,10 @@
         <v>2725709</v>
       </c>
       <c r="H77" s="51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I77" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J77" s="49">
         <v>1.8594732384912049</v>
@@ -8643,10 +8722,10 @@
     <row r="78" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="30"/>
       <c r="B78" s="54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C78" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D78" s="49">
         <v>1.9530798172427088</v>
@@ -8658,10 +8737,10 @@
         <v>2826096</v>
       </c>
       <c r="H78" s="51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I78" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J78" s="49">
         <v>1.892198034308179</v>
@@ -8673,10 +8752,10 @@
     <row r="79" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="30"/>
       <c r="B79" s="47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D79" s="42">
         <v>2.0005459598703146</v>
@@ -8688,10 +8767,10 @@
         <v>2931334</v>
       </c>
       <c r="H79" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I79" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J79" s="42">
         <v>2.0003592159356653</v>
@@ -8703,7 +8782,7 @@
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="30"/>
       <c r="B80" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C80" s="39"/>
       <c r="D80" s="38"/>
@@ -8714,111 +8793,111 @@
     <row r="81" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="30"/>
       <c r="B81" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C81" s="95" t="s">
-        <v>211</v>
-      </c>
-      <c r="D81" s="95"/>
-      <c r="E81" s="95"/>
-      <c r="F81" s="95"/>
-      <c r="G81" s="95"/>
-      <c r="H81" s="95"/>
-      <c r="I81" s="95"/>
-      <c r="J81" s="95"/>
-      <c r="K81" s="95"/>
+        <v>39</v>
+      </c>
+      <c r="C81" s="94" t="s">
+        <v>210</v>
+      </c>
+      <c r="D81" s="94"/>
+      <c r="E81" s="94"/>
+      <c r="F81" s="94"/>
+      <c r="G81" s="94"/>
+      <c r="H81" s="94"/>
+      <c r="I81" s="94"/>
+      <c r="J81" s="94"/>
+      <c r="K81" s="94"/>
     </row>
     <row r="82" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="30"/>
       <c r="B82" s="32"/>
-      <c r="C82" s="106" t="s">
-        <v>206</v>
-      </c>
-      <c r="D82" s="95"/>
-      <c r="E82" s="95"/>
-      <c r="F82" s="95"/>
-      <c r="G82" s="95"/>
-      <c r="H82" s="95"/>
-      <c r="I82" s="95"/>
-      <c r="J82" s="95"/>
-      <c r="K82" s="95"/>
+      <c r="C82" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="94"/>
+      <c r="E82" s="94"/>
+      <c r="F82" s="94"/>
+      <c r="G82" s="94"/>
+      <c r="H82" s="94"/>
+      <c r="I82" s="94"/>
+      <c r="J82" s="94"/>
+      <c r="K82" s="94"/>
     </row>
     <row r="83" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="30"/>
       <c r="B83" s="32"/>
-      <c r="C83" s="95" t="s">
-        <v>210</v>
-      </c>
-      <c r="D83" s="95"/>
-      <c r="E83" s="95"/>
-      <c r="F83" s="95"/>
-      <c r="G83" s="95"/>
-      <c r="H83" s="95"/>
-      <c r="I83" s="95"/>
-      <c r="J83" s="95"/>
-      <c r="K83" s="95"/>
+      <c r="C83" s="94" t="s">
+        <v>209</v>
+      </c>
+      <c r="D83" s="94"/>
+      <c r="E83" s="94"/>
+      <c r="F83" s="94"/>
+      <c r="G83" s="94"/>
+      <c r="H83" s="94"/>
+      <c r="I83" s="94"/>
+      <c r="J83" s="94"/>
+      <c r="K83" s="94"/>
     </row>
     <row r="84" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="30"/>
       <c r="B84" s="32"/>
-      <c r="C84" s="106" t="s">
-        <v>206</v>
-      </c>
-      <c r="D84" s="95"/>
-      <c r="E84" s="95"/>
-      <c r="F84" s="95"/>
-      <c r="G84" s="95"/>
-      <c r="H84" s="95"/>
-      <c r="I84" s="95"/>
-      <c r="J84" s="95"/>
-      <c r="K84" s="95"/>
+      <c r="C84" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D84" s="94"/>
+      <c r="E84" s="94"/>
+      <c r="F84" s="94"/>
+      <c r="G84" s="94"/>
+      <c r="H84" s="94"/>
+      <c r="I84" s="94"/>
+      <c r="J84" s="94"/>
+      <c r="K84" s="94"/>
     </row>
     <row r="85" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="30"/>
       <c r="B85" s="32"/>
-      <c r="C85" s="107" t="s">
-        <v>209</v>
-      </c>
-      <c r="D85" s="107"/>
-      <c r="E85" s="107"/>
-      <c r="F85" s="107"/>
-      <c r="G85" s="107"/>
-      <c r="H85" s="107"/>
-      <c r="I85" s="107"/>
-      <c r="J85" s="107"/>
-      <c r="K85" s="107"/>
+      <c r="C85" s="106" t="s">
+        <v>208</v>
+      </c>
+      <c r="D85" s="106"/>
+      <c r="E85" s="106"/>
+      <c r="F85" s="106"/>
+      <c r="G85" s="106"/>
+      <c r="H85" s="106"/>
+      <c r="I85" s="106"/>
+      <c r="J85" s="106"/>
+      <c r="K85" s="106"/>
     </row>
     <row r="86" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="30"/>
       <c r="B86" s="32"/>
-      <c r="C86" s="106" t="s">
-        <v>198</v>
-      </c>
-      <c r="D86" s="95"/>
-      <c r="E86" s="95"/>
-      <c r="F86" s="95"/>
-      <c r="G86" s="95"/>
-      <c r="H86" s="95"/>
-      <c r="I86" s="95"/>
-      <c r="J86" s="95"/>
-      <c r="K86" s="95"/>
+      <c r="C86" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="D86" s="94"/>
+      <c r="E86" s="94"/>
+      <c r="F86" s="94"/>
+      <c r="G86" s="94"/>
+      <c r="H86" s="94"/>
+      <c r="I86" s="94"/>
+      <c r="J86" s="94"/>
+      <c r="K86" s="94"/>
     </row>
     <row r="87" spans="1:16" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="30"/>
       <c r="B87" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="95" t="s">
-        <v>208</v>
-      </c>
-      <c r="D87" s="95"/>
-      <c r="E87" s="95"/>
-      <c r="F87" s="95"/>
-      <c r="G87" s="95"/>
-      <c r="H87" s="95"/>
-      <c r="I87" s="95"/>
-      <c r="J87" s="95"/>
-      <c r="K87" s="95"/>
+        <v>38</v>
+      </c>
+      <c r="C87" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" s="94"/>
+      <c r="E87" s="94"/>
+      <c r="F87" s="94"/>
+      <c r="G87" s="94"/>
+      <c r="H87" s="94"/>
+      <c r="I87" s="94"/>
+      <c r="J87" s="94"/>
+      <c r="K87" s="94"/>
       <c r="M87" s="31"/>
       <c r="N87" s="31"/>
       <c r="P87" s="31"/>
@@ -8826,32 +8905,32 @@
     <row r="88" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
       <c r="B88" s="32"/>
-      <c r="C88" s="106" t="s">
-        <v>206</v>
-      </c>
-      <c r="D88" s="95"/>
-      <c r="E88" s="95"/>
-      <c r="F88" s="95"/>
-      <c r="G88" s="95"/>
-      <c r="H88" s="95"/>
-      <c r="I88" s="95"/>
-      <c r="J88" s="95"/>
-      <c r="K88" s="95"/>
+      <c r="C88" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D88" s="94"/>
+      <c r="E88" s="94"/>
+      <c r="F88" s="94"/>
+      <c r="G88" s="94"/>
+      <c r="H88" s="94"/>
+      <c r="I88" s="94"/>
+      <c r="J88" s="94"/>
+      <c r="K88" s="94"/>
     </row>
     <row r="89" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="30"/>
       <c r="B89" s="32"/>
-      <c r="C89" s="95" t="s">
-        <v>207</v>
-      </c>
-      <c r="D89" s="95"/>
-      <c r="E89" s="95"/>
-      <c r="F89" s="95"/>
-      <c r="G89" s="95"/>
-      <c r="H89" s="95"/>
-      <c r="I89" s="95"/>
-      <c r="J89" s="95"/>
-      <c r="K89" s="95"/>
+      <c r="C89" s="94" t="s">
+        <v>206</v>
+      </c>
+      <c r="D89" s="94"/>
+      <c r="E89" s="94"/>
+      <c r="F89" s="94"/>
+      <c r="G89" s="94"/>
+      <c r="H89" s="94"/>
+      <c r="I89" s="94"/>
+      <c r="J89" s="94"/>
+      <c r="K89" s="94"/>
       <c r="M89" s="31"/>
       <c r="N89" s="31"/>
       <c r="P89" s="31"/>
@@ -8859,52 +8938,52 @@
     <row r="90" spans="1:16" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="30"/>
       <c r="B90" s="32"/>
-      <c r="C90" s="106" t="s">
-        <v>206</v>
-      </c>
-      <c r="D90" s="95"/>
-      <c r="E90" s="95"/>
-      <c r="F90" s="95"/>
-      <c r="G90" s="95"/>
-      <c r="H90" s="95"/>
-      <c r="I90" s="95"/>
-      <c r="J90" s="95"/>
-      <c r="K90" s="95"/>
+      <c r="C90" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D90" s="94"/>
+      <c r="E90" s="94"/>
+      <c r="F90" s="94"/>
+      <c r="G90" s="94"/>
+      <c r="H90" s="94"/>
+      <c r="I90" s="94"/>
+      <c r="J90" s="94"/>
+      <c r="K90" s="94"/>
     </row>
     <row r="91" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="30"/>
       <c r="B91" s="32"/>
-      <c r="C91" s="107" t="s">
-        <v>205</v>
-      </c>
-      <c r="D91" s="107"/>
-      <c r="E91" s="107"/>
-      <c r="F91" s="107"/>
-      <c r="G91" s="107"/>
-      <c r="H91" s="107"/>
-      <c r="I91" s="107"/>
-      <c r="J91" s="107"/>
-      <c r="K91" s="107"/>
+      <c r="C91" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="D91" s="106"/>
+      <c r="E91" s="106"/>
+      <c r="F91" s="106"/>
+      <c r="G91" s="106"/>
+      <c r="H91" s="106"/>
+      <c r="I91" s="106"/>
+      <c r="J91" s="106"/>
+      <c r="K91" s="106"/>
     </row>
     <row r="92" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="30"/>
       <c r="B92" s="32"/>
-      <c r="C92" s="106" t="s">
-        <v>198</v>
-      </c>
-      <c r="D92" s="95"/>
-      <c r="E92" s="95"/>
-      <c r="F92" s="95"/>
-      <c r="G92" s="95"/>
-      <c r="H92" s="95"/>
-      <c r="I92" s="95"/>
-      <c r="J92" s="95"/>
-      <c r="K92" s="95"/>
+      <c r="C92" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="D92" s="94"/>
+      <c r="E92" s="94"/>
+      <c r="F92" s="94"/>
+      <c r="G92" s="94"/>
+      <c r="H92" s="94"/>
+      <c r="I92" s="94"/>
+      <c r="J92" s="94"/>
+      <c r="K92" s="94"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="30"/>
       <c r="B93" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C93" s="31"/>
       <c r="D93" s="35"/>
@@ -8918,95 +8997,95 @@
     </row>
     <row r="94" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C94" s="108" t="s">
-        <v>204</v>
-      </c>
-      <c r="D94" s="108"/>
-      <c r="E94" s="108"/>
-      <c r="F94" s="108"/>
-      <c r="G94" s="108"/>
-      <c r="H94" s="108"/>
-      <c r="I94" s="108"/>
-      <c r="J94" s="108"/>
-      <c r="K94" s="108"/>
+        <v>36</v>
+      </c>
+      <c r="C94" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="D94" s="107"/>
+      <c r="E94" s="107"/>
+      <c r="F94" s="107"/>
+      <c r="G94" s="107"/>
+      <c r="H94" s="107"/>
+      <c r="I94" s="107"/>
+      <c r="J94" s="107"/>
+      <c r="K94" s="107"/>
       <c r="M94" s="31"/>
       <c r="N94" s="31"/>
       <c r="P94" s="31"/>
     </row>
     <row r="95" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B95" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C95" s="95" t="s">
-        <v>203</v>
-      </c>
-      <c r="D95" s="95"/>
-      <c r="E95" s="95"/>
-      <c r="F95" s="95"/>
-      <c r="G95" s="95"/>
-      <c r="H95" s="95"/>
-      <c r="I95" s="95"/>
-      <c r="J95" s="95"/>
-      <c r="K95" s="95"/>
+        <v>35</v>
+      </c>
+      <c r="C95" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="D95" s="94"/>
+      <c r="E95" s="94"/>
+      <c r="F95" s="94"/>
+      <c r="G95" s="94"/>
+      <c r="H95" s="94"/>
+      <c r="I95" s="94"/>
+      <c r="J95" s="94"/>
+      <c r="K95" s="94"/>
       <c r="M95" s="31"/>
       <c r="N95" s="31"/>
       <c r="P95" s="31"/>
     </row>
     <row r="96" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C96" s="95" t="s">
-        <v>202</v>
-      </c>
-      <c r="D96" s="95"/>
-      <c r="E96" s="95"/>
-      <c r="F96" s="95"/>
-      <c r="G96" s="95"/>
-      <c r="H96" s="95"/>
-      <c r="I96" s="95"/>
-      <c r="J96" s="95"/>
-      <c r="K96" s="95"/>
+        <v>34</v>
+      </c>
+      <c r="C96" s="94" t="s">
+        <v>201</v>
+      </c>
+      <c r="D96" s="94"/>
+      <c r="E96" s="94"/>
+      <c r="F96" s="94"/>
+      <c r="G96" s="94"/>
+      <c r="H96" s="94"/>
+      <c r="I96" s="94"/>
+      <c r="J96" s="94"/>
+      <c r="K96" s="94"/>
       <c r="M96" s="31"/>
       <c r="N96" s="31"/>
       <c r="P96" s="31"/>
     </row>
     <row r="97" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C97" s="95" t="s">
-        <v>201</v>
-      </c>
-      <c r="D97" s="95"/>
-      <c r="E97" s="95"/>
-      <c r="F97" s="95"/>
-      <c r="G97" s="95"/>
-      <c r="H97" s="95"/>
-      <c r="I97" s="95"/>
-      <c r="J97" s="95"/>
-      <c r="K97" s="95"/>
+        <v>33</v>
+      </c>
+      <c r="C97" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="D97" s="94"/>
+      <c r="E97" s="94"/>
+      <c r="F97" s="94"/>
+      <c r="G97" s="94"/>
+      <c r="H97" s="94"/>
+      <c r="I97" s="94"/>
+      <c r="J97" s="94"/>
+      <c r="K97" s="94"/>
       <c r="M97" s="31"/>
       <c r="N97" s="31"/>
       <c r="P97" s="31"/>
     </row>
     <row r="98" spans="1:16" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C98" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="D98" s="95"/>
-      <c r="E98" s="95"/>
-      <c r="F98" s="95"/>
-      <c r="G98" s="95"/>
-      <c r="H98" s="95"/>
-      <c r="I98" s="95"/>
-      <c r="J98" s="95"/>
-      <c r="K98" s="95"/>
+      <c r="C98" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" s="94"/>
+      <c r="E98" s="94"/>
+      <c r="F98" s="94"/>
+      <c r="G98" s="94"/>
+      <c r="H98" s="94"/>
+      <c r="I98" s="94"/>
+      <c r="J98" s="94"/>
+      <c r="K98" s="94"/>
       <c r="M98" s="31"/>
       <c r="N98" s="31"/>
       <c r="P98" s="31"/>
@@ -9014,36 +9093,36 @@
     <row r="99" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="30"/>
       <c r="B99" s="32"/>
-      <c r="C99" s="106" t="s">
-        <v>31</v>
-      </c>
-      <c r="D99" s="95"/>
-      <c r="E99" s="95"/>
-      <c r="F99" s="95"/>
-      <c r="G99" s="95"/>
-      <c r="H99" s="95"/>
-      <c r="I99" s="95"/>
-      <c r="J99" s="95"/>
-      <c r="K99" s="95"/>
+      <c r="C99" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" s="94"/>
+      <c r="E99" s="94"/>
+      <c r="F99" s="94"/>
+      <c r="G99" s="94"/>
+      <c r="H99" s="94"/>
+      <c r="I99" s="94"/>
+      <c r="J99" s="94"/>
+      <c r="K99" s="94"/>
       <c r="M99" s="31"/>
       <c r="N99" s="31"/>
       <c r="P99" s="31"/>
     </row>
     <row r="100" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B100" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C100" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="95"/>
-      <c r="E100" s="95"/>
-      <c r="F100" s="95"/>
-      <c r="G100" s="95"/>
-      <c r="H100" s="95"/>
-      <c r="I100" s="95"/>
-      <c r="J100" s="95"/>
-      <c r="K100" s="95"/>
+      <c r="C100" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="D100" s="94"/>
+      <c r="E100" s="94"/>
+      <c r="F100" s="94"/>
+      <c r="G100" s="94"/>
+      <c r="H100" s="94"/>
+      <c r="I100" s="94"/>
+      <c r="J100" s="94"/>
+      <c r="K100" s="94"/>
       <c r="M100" s="31"/>
       <c r="N100" s="31"/>
       <c r="P100" s="31"/>
@@ -9051,17 +9130,17 @@
     <row r="101" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="30"/>
       <c r="B101" s="32"/>
-      <c r="C101" s="106" t="s">
-        <v>28</v>
-      </c>
-      <c r="D101" s="95"/>
-      <c r="E101" s="95"/>
-      <c r="F101" s="95"/>
-      <c r="G101" s="95"/>
-      <c r="H101" s="95"/>
-      <c r="I101" s="95"/>
-      <c r="J101" s="95"/>
-      <c r="K101" s="95"/>
+      <c r="C101" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="94"/>
+      <c r="E101" s="94"/>
+      <c r="F101" s="94"/>
+      <c r="G101" s="94"/>
+      <c r="H101" s="94"/>
+      <c r="I101" s="94"/>
+      <c r="J101" s="94"/>
+      <c r="K101" s="94"/>
       <c r="M101" s="31"/>
       <c r="N101" s="31"/>
       <c r="P101" s="31"/>

</xml_diff>